<commit_message>
6a was not correct
</commit_message>
<xml_diff>
--- a/Klass 6a.xlsx
+++ b/Klass 6a.xlsx
@@ -453,7 +453,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -547,7 +547,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -561,7 +561,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -575,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -589,7 +589,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -603,7 +603,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -617,7 +617,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -631,7 +631,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -645,7 +645,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -687,7 +687,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>7</v>
@@ -715,7 +715,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>6</v>

</xml_diff>